<commit_message>
Added logo, front copper fills, rerouting and model number. Updated BOM file
</commit_message>
<xml_diff>
--- a/sparrow_v1_BOM_global.xlsx
+++ b/sparrow_v1_BOM_global.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pollock\Documents\Repo\quark_pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F194C735-B9D9-4E72-9FBD-E5601570B0D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E93B3BB-7D48-475D-A19D-9436380EDF2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2070" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>22 uF/10V (20%)</t>
-  </si>
-  <si>
-    <t>0603</t>
   </si>
   <si>
     <t>Capacitor</t>
@@ -205,6 +202,9 @@
   </si>
   <si>
     <t>2.54mm Pitch Male Pin Header Connector Strip Pin Connectors Adaptor</t>
+  </si>
+  <si>
+    <t>1206</t>
   </si>
 </sst>
 </file>
@@ -252,7 +252,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,6 +271,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -379,8 +391,68 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -393,65 +465,25 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,7 +768,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -748,315 +780,319 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="26.4">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="9">
+      <c r="B3" s="5">
         <v>2</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="11" t="s">
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" s="5">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="B4" s="9">
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="29"/>
+      <c r="B7" s="30">
         <v>4</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="B5" s="9">
+      <c r="C7" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="25"/>
+      <c r="B8" s="26">
         <v>1</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="C8" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="11" t="s">
+      <c r="G8" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="B6" s="9">
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26">
         <v>1</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="C9" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" s="9">
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="25"/>
+      <c r="B10" s="26">
         <v>4</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C10" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="11" t="s">
+      <c r="E10" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="9">
+    </row>
+    <row r="11" spans="1:7" ht="40.200000000000003" thickBot="1">
+      <c r="B11" s="10">
         <v>1</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" s="9">
+      <c r="C11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" s="6">
         <v>1</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="9">
-        <v>4</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="119.4" thickBot="1">
-      <c r="B11" s="14">
+      <c r="C12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" s="10">
+      <c r="C13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="6">
         <v>1</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="B13" s="10">
+      <c r="C14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="5">
         <v>1</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="B14" s="10">
-        <v>1</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="11" t="s">
+      <c r="C15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="9">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="E15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="F15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="G15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="11" t="s">
+    </row>
+    <row r="16" spans="1:7" ht="26.4">
+      <c r="B16" s="15">
+        <v>2</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="26.4">
-      <c r="B16" s="19">
-        <v>2</v>
-      </c>
-      <c r="C16" s="24" t="s">
+      <c r="D16" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="E16" s="17"/>
+      <c r="F16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="18" t="s">
         <v>52</v>
-      </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOM file with PWR2 and gerber files
</commit_message>
<xml_diff>
--- a/sparrow_v1_BOM_global.xlsx
+++ b/sparrow_v1_BOM_global.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pollock\Documents\Repo\quark_pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E93B3BB-7D48-475D-A19D-9436380EDF2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47D3154-164A-4C3D-8AB9-7D3EE090C0CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2070" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -206,12 +206,24 @@
   <si>
     <t>1206</t>
   </si>
+  <si>
+    <t>J7 (PWR2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JST XH2.54 2 Pin </t>
+  </si>
+  <si>
+    <t>Pitch 2.54 Male Connector PCB mounter</t>
+  </si>
+  <si>
+    <t>https://www.google.com/imgres?imgurl=https%3A%2F%2Fprotosupplies.com%2Fwp-content%2Fuploads%2F2019%2F06%2FJST-XH-2.54-2-pin-Male-Connector-5-Pack.jpg&amp;imgrefurl=https%3A%2F%2Fprotosupplies.com%2Fproduct%2Fjst-xh2-54-2-pin-male-connector-5-pack%2F&amp;docid=EzBjSRWFGcd9OM&amp;tbnid=Tez_QMMvEgBigM%3A&amp;vet=10ahUKEwiX4bTl1_vlAhUbzjgGHZ8ABuIQMwhgKAkwCQ..i&amp;w=800&amp;h=600&amp;bih=920&amp;biw=1920&amp;q=jst%202%20pin%20male%20connector%20pcb&amp;ved=0ahUKEwiX4bTl1_vlAhUbzjgGHZ8ABuIQMwhgKAkwCQ&amp;iact=mrc&amp;uact=8</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +262,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -388,10 +408,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -453,6 +474,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -465,28 +506,13 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -765,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -780,15 +806,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
@@ -894,86 +920,86 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="29"/>
-      <c r="B7" s="30">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26">
         <v>4</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="27" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26">
+      <c r="A8" s="21"/>
+      <c r="B8" s="22">
         <v>1</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26">
+      <c r="A9" s="21"/>
+      <c r="B9" s="22">
         <v>1</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26">
+      <c r="A10" s="21"/>
+      <c r="B10" s="22">
         <v>4</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="23" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1093,12 +1119,32 @@
       </c>
       <c r="G16" s="18" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8">
+      <c r="C17" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H17" r:id="rId1" display="https://www.google.com/imgres?imgurl=https%3A%2F%2Fprotosupplies.com%2Fwp-content%2Fuploads%2F2019%2F06%2FJST-XH-2.54-2-pin-Male-Connector-5-Pack.jpg&amp;imgrefurl=https%3A%2F%2Fprotosupplies.com%2Fproduct%2Fjst-xh2-54-2-pin-male-connector-5-pack%2F&amp;docid=EzBjSRWFGcd9OM&amp;tbnid=Tez_QMMvEgBigM%3A&amp;vet=10ahUKEwiX4bTl1_vlAhUbzjgGHZ8ABuIQMwhgKAkwCQ..i&amp;w=800&amp;h=600&amp;bih=920&amp;biw=1920&amp;q=jst%202%20pin%20male%20connector%20pcb&amp;ved=0ahUKEwiX4bTl1_vlAhUbzjgGHZ8ABuIQMwhgKAkwCQ&amp;iact=mrc&amp;uact=8" xr:uid="{6FC40758-F671-45A2-A521-FF8C10F9562B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>